<commit_message>
pick and sort v0.3
</commit_message>
<xml_diff>
--- a/QtDesigner/demo2_openfile/utils/7月未申报0716.xlsx
+++ b/QtDesigner/demo2_openfile/utils/7月未申报0716.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13140" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="829">
   <si>
     <t>社会信用代码（纳税人识别号）</t>
   </si>
@@ -2496,19 +2496,16 @@
     <t>北京市昌平区沙河镇满井东队</t>
   </si>
   <si>
-    <t>未申报查询</t>
+    <t>税务所</t>
+  </si>
+  <si>
+    <t>一所</t>
   </si>
   <si>
     <t>制表人：zol.com.cn</t>
   </si>
   <si>
-    <t>税务所</t>
-  </si>
-  <si>
     <t>沙河</t>
-  </si>
-  <si>
-    <t>一所</t>
   </si>
 </sst>
 </file>
@@ -2517,9 +2514,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -2542,15 +2539,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2571,9 +2567,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2587,14 +2582,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -2602,6 +2589,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -2611,7 +2599,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2625,9 +2613,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2655,6 +2642,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
@@ -2664,21 +2667,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2693,25 +2690,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2732,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2771,19 +2780,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2819,61 +2840,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2967,6 +2964,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2982,26 +2997,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3032,17 +3038,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.399975585192419"/>
@@ -3051,25 +3046,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3081,10 +3078,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3093,31 +3090,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3126,104 +3123,104 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3256,9 +3253,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -4623,40 +4617,40 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="16" t="s">
+      <c r="C29" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G29" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="I29" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="J29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="L29" s="17"/>
+      <c r="J29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="16"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="11.25" spans="1:12">
       <c r="A30" s="8" t="s">
@@ -9901,10 +9895,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M2:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -9912,66 +9906,92 @@
     <col min="1" max="1" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="14" t="s">
+    <row r="1" s="1" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" ht="11.25" spans="1:12">
+    </row>
+    <row r="2" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A3" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -9983,16 +10003,16 @@
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>20</v>
@@ -10001,16 +10021,19 @@
         <v>21</v>
       </c>
       <c r="L3" s="13"/>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M3" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A4" s="8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
@@ -10019,31 +10042,36 @@
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="13"/>
-    </row>
-    <row r="5" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="L4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A5" s="8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
@@ -10055,16 +10083,16 @@
         <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>32</v>
@@ -10073,15 +10101,18 @@
         <v>21</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="11.25" spans="1:12">
+        <v>39</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A6" s="8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>28</v>
@@ -10093,16 +10124,16 @@
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>32</v>
@@ -10113,13 +10144,16 @@
       <c r="L6" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M6" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>28</v>
@@ -10131,16 +10165,16 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>32</v>
@@ -10151,85 +10185,94 @@
       <c r="L7" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M7" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:13">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" s="2" customFormat="1" spans="1:12">
-      <c r="A9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="K9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="13"/>
-    </row>
-    <row r="10" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="L9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A10" s="8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>28</v>
@@ -10241,16 +10284,16 @@
         <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>32</v>
@@ -10259,375 +10302,408 @@
         <v>21</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="11.25" spans="1:12">
+        <v>39</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A11" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:13">
+      <c r="A13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="13" t="s">
+      <c r="K14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="13"/>
-    </row>
-    <row r="13" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="13"/>
-    </row>
-    <row r="14" s="2" customFormat="1" spans="1:12">
-      <c r="A14" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M14" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A15" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="13"/>
+      <c r="M15" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:13">
+      <c r="A16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="M16" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="M17" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="18" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="M18" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A19" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J15" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="13" t="s">
+      <c r="K20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A16" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="13"/>
-    </row>
-    <row r="17" s="2" customFormat="1" spans="1:12">
-      <c r="A17" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="13"/>
-    </row>
-    <row r="18" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A18" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="13"/>
-    </row>
-    <row r="19" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A19" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A20" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="13"/>
-    </row>
-    <row r="21" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M20" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A21" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>28</v>
@@ -10639,16 +10715,16 @@
         <v>16</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>32</v>
@@ -10659,90 +10735,99 @@
       <c r="L21" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M21" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A22" s="8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="13"/>
+      <c r="M22" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="23" s="2" customFormat="1" ht="11.25" spans="1:13">
+      <c r="A23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J22" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="13" t="s">
+      <c r="K23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A23" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="13"/>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="M23" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A24" s="8" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>15</v>
@@ -10751,33 +10836,34 @@
         <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="11.25" spans="1:12">
+      <c r="L24" s="13"/>
+      <c r="M24" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="25" s="2" customFormat="1" ht="11.25" spans="1:13">
       <c r="A25" s="8" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>14</v>
@@ -10789,16 +10875,16 @@
         <v>16</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>20</v>
@@ -10807,52 +10893,18 @@
         <v>21</v>
       </c>
       <c r="L25" s="13"/>
-    </row>
-    <row r="26" s="2" customFormat="1" ht="11.25" spans="1:12">
-      <c r="A26" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="M25" s="2" t="s">
         <v>826</v>
       </c>
     </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>827</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A27:L27"/>
+  <mergeCells count="1">
+    <mergeCell ref="A26:L26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -10864,8 +10916,8 @@
   <sheetPr/>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -10908,7 +10960,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="11.25" spans="1:12">
@@ -11492,7 +11544,7 @@
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" spans="1:13">
@@ -11529,7 +11581,7 @@
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11568,7 +11620,7 @@
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11607,7 +11659,7 @@
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11646,7 +11698,7 @@
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11687,7 +11739,7 @@
         <v>39</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11728,7 +11780,7 @@
         <v>39</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11767,7 +11819,7 @@
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11808,7 +11860,7 @@
         <v>39</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11847,7 +11899,7 @@
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="11.25" spans="1:13">
@@ -11886,7 +11938,7 @@
       </c>
       <c r="L27" s="13"/>
       <c r="M27" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>